<commit_message>
Added validation files for information and jurisdiction ontology
</commit_message>
<xml_diff>
--- a/ontology/ontology_prototype/Excel/Object Properties.xlsx
+++ b/ontology/ontology_prototype/Excel/Object Properties.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Uni\Master\Master Thesis\Repository\devotigdl\ontology\ontology_prototype\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8E6B412-F77D-4374-B55C-B0D7F184C1FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7783C3FB-4B43-49FB-A735-C33399F207B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" activeTab="2" xr2:uid="{FF477061-936F-4B4B-A8AE-438439C0BE71}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18645" windowHeight="21000" activeTab="3" xr2:uid="{FF477061-936F-4B4B-A8AE-438439C0BE71}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction Object Properties" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="751" uniqueCount="260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="761" uniqueCount="263">
   <si>
     <t>Subproperty</t>
   </si>
@@ -819,6 +819,15 @@
   </si>
   <si>
     <t>OrganizationUnit</t>
+  </si>
+  <si>
+    <t>responsibleForTool</t>
+  </si>
+  <si>
+    <t>responsibleFor</t>
+  </si>
+  <si>
+    <t>createdsData</t>
   </si>
 </sst>
 </file>
@@ -834,7 +843,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -856,6 +865,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1007,7 +1022,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -1021,13 +1036,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
@@ -1035,6 +1044,8 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1903,53 +1914,53 @@
       <c r="E2" s="2"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="D3" s="14" t="s">
+      <c r="D3" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="E3" s="13" t="s">
+      <c r="E3" s="1" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C4" s="13" t="s">
+      <c r="C4" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="D4" s="14" t="s">
+      <c r="D4" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="E4" s="13" t="s">
+      <c r="E4" s="1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="13" t="s">
+      <c r="A5" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B5" s="13" t="s">
+      <c r="B5" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C5" s="13" t="s">
+      <c r="C5" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="D5" s="14" t="s">
+      <c r="D5" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="E5" s="13" t="s">
+      <c r="E5" s="1" t="s">
         <v>9</v>
       </c>
     </row>
@@ -2005,18 +2016,18 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="13"/>
-      <c r="B9" s="13"/>
-      <c r="C9" s="13"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="13"/>
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="1"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="13"/>
-      <c r="B10" s="13"/>
-      <c r="C10" s="13"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="13"/>
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -2027,7 +2038,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22FDCA7C-E0FF-452B-9441-D42FFE281F20}">
   <dimension ref="A1:E62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+    <sheetView topLeftCell="A11" workbookViewId="0">
       <selection activeCell="C76" sqref="C76"/>
     </sheetView>
   </sheetViews>
@@ -2040,938 +2051,938 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="22" t="s">
+      <c r="D1" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="21" t="s">
+      <c r="E1" s="15" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="C2" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="D2" s="16" t="s">
+      <c r="D2" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="E2" s="16" t="s">
+      <c r="E2" s="1" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="C3" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="D3" s="16" t="s">
+      <c r="D3" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="E3" s="16" t="s">
+      <c r="E3" s="1" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="16" t="s">
+      <c r="A4" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B4" s="16" t="s">
+      <c r="B4" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="C4" s="16" t="s">
+      <c r="C4" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="D4" s="16" t="s">
+      <c r="D4" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="E4" s="16" t="s">
+      <c r="E4" s="1" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="16" t="s">
+      <c r="A5" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="B5" s="16" t="s">
+      <c r="B5" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C5" s="16" t="s">
+      <c r="C5" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="D5" s="16" t="s">
+      <c r="D5" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="E5" s="16" t="s">
+      <c r="E5" s="1" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="16" t="s">
+      <c r="A6" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B6" s="16" t="s">
+      <c r="B6" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="C6" s="16" t="s">
+      <c r="C6" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="D6" s="16" t="s">
+      <c r="D6" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="E6" s="16" t="s">
+      <c r="E6" s="1" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="16" t="s">
+      <c r="A7" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="B7" s="16" t="s">
+      <c r="B7" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="C7" s="16" t="s">
+      <c r="C7" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="D7" s="16" t="s">
+      <c r="D7" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="E7" s="16" t="s">
+      <c r="E7" s="1" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="16" t="s">
+      <c r="A8" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="B8" s="16" t="s">
+      <c r="B8" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="C8" s="16" t="s">
+      <c r="C8" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="D8" s="16" t="s">
+      <c r="D8" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="E8" s="16" t="s">
+      <c r="E8" s="1" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="16" t="s">
+      <c r="A9" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B9" s="16" t="s">
+      <c r="B9" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="C9" s="16" t="s">
+      <c r="C9" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="D9" s="16" t="s">
+      <c r="D9" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="E9" s="16" t="s">
+      <c r="E9" s="1" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="16" t="s">
+      <c r="A10" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="B10" s="16" t="s">
+      <c r="B10" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="C10" s="16" t="s">
+      <c r="C10" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="D10" s="16" t="s">
+      <c r="D10" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="E10" s="16" t="s">
+      <c r="E10" s="1" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="16" t="s">
+      <c r="A11" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="B11" s="16" t="s">
+      <c r="B11" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="C11" s="16" t="s">
+      <c r="C11" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="D11" s="16" t="s">
+      <c r="D11" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="E11" s="16" t="s">
+      <c r="E11" s="1" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="16" t="s">
+      <c r="A12" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="B12" s="16" t="s">
+      <c r="B12" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="C12" s="16" t="s">
+      <c r="C12" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="D12" s="16" t="s">
+      <c r="D12" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="E12" s="16" t="s">
+      <c r="E12" s="1" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="16"/>
-      <c r="B13" s="16"/>
-      <c r="C13" s="16"/>
-      <c r="D13" s="16" t="s">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="E13" s="16" t="s">
+      <c r="E13" s="1" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="16" t="s">
+      <c r="A14" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="B14" s="16" t="s">
+      <c r="B14" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="C14" s="16" t="s">
+      <c r="C14" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="D14" s="16" t="s">
+      <c r="D14" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="E14" s="16" t="s">
+      <c r="E14" s="1" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="16"/>
-      <c r="B15" s="16"/>
-      <c r="C15" s="16"/>
-      <c r="D15" s="16" t="s">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="E15" s="16" t="s">
+      <c r="E15" s="1" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="16" t="s">
+      <c r="A16" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="B16" s="16" t="s">
+      <c r="B16" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C16" s="16" t="s">
+      <c r="C16" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="D16" s="16" t="s">
+      <c r="D16" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="E16" s="16" t="s">
+      <c r="E16" s="1" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="16"/>
-      <c r="B17" s="16"/>
-      <c r="C17" s="16"/>
-      <c r="D17" s="16" t="s">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="E17" s="16" t="s">
+      <c r="E17" s="1" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="16" t="s">
+      <c r="A18" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="B18" s="16" t="s">
+      <c r="B18" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C18" s="16" t="s">
+      <c r="C18" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="D18" s="16" t="s">
+      <c r="D18" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="E18" s="16" t="s">
+      <c r="E18" s="1" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="16"/>
-      <c r="B19" s="16"/>
-      <c r="C19" s="16"/>
-      <c r="D19" s="16" t="s">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="E19" s="16" t="s">
+      <c r="E19" s="1" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="16" t="s">
+      <c r="A20" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="B20" s="16" t="s">
+      <c r="B20" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C20" s="16" t="s">
+      <c r="C20" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="D20" s="16" t="s">
+      <c r="D20" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="E20" s="16" t="s">
+      <c r="E20" s="1" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="16"/>
-      <c r="B21" s="16"/>
-      <c r="C21" s="16"/>
-      <c r="D21" s="16" t="s">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="E21" s="16" t="s">
+      <c r="E21" s="1" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="16" t="s">
+      <c r="A22" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="B22" s="16" t="s">
+      <c r="B22" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="C22" s="16" t="s">
+      <c r="C22" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="D22" s="16" t="s">
+      <c r="D22" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="E22" s="16" t="s">
+      <c r="E22" s="1" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="16"/>
-      <c r="B23" s="16"/>
-      <c r="C23" s="16"/>
-      <c r="D23" s="16" t="s">
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="E23" s="16" t="s">
+      <c r="E23" s="1" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="16" t="s">
+      <c r="A24" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="B24" s="16" t="s">
+      <c r="B24" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="C24" s="16" t="s">
+      <c r="C24" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="D24" s="16" t="s">
+      <c r="D24" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="E24" s="16" t="s">
+      <c r="E24" s="1" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="16"/>
-      <c r="B25" s="16"/>
-      <c r="C25" s="16"/>
-      <c r="D25" s="16" t="s">
+      <c r="A25" s="1"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="E25" s="16" t="s">
+      <c r="E25" s="1" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="16" t="s">
+      <c r="A26" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="B26" s="16" t="s">
+      <c r="B26" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="C26" s="16" t="s">
+      <c r="C26" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="D26" s="16" t="s">
+      <c r="D26" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="E26" s="16" t="s">
+      <c r="E26" s="1" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="16"/>
-      <c r="B27" s="16"/>
-      <c r="C27" s="16"/>
-      <c r="D27" s="16" t="s">
+      <c r="A27" s="1"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="E27" s="16" t="s">
+      <c r="E27" s="1" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="16" t="s">
+      <c r="A28" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="B28" s="16" t="s">
+      <c r="B28" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="C28" s="16" t="s">
+      <c r="C28" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="D28" s="23"/>
-      <c r="E28" s="16" t="s">
+      <c r="D28" s="17"/>
+      <c r="E28" s="1" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="24" t="s">
+      <c r="A29" s="18" t="s">
         <v>115</v>
       </c>
-      <c r="B29" s="24" t="s">
+      <c r="B29" s="18" t="s">
         <v>108</v>
       </c>
-      <c r="C29" s="24" t="s">
+      <c r="C29" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="D29" s="24" t="s">
+      <c r="D29" s="18" t="s">
         <v>116</v>
       </c>
-      <c r="E29" s="24" t="s">
+      <c r="E29" s="18" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="24"/>
-      <c r="B30" s="24"/>
-      <c r="C30" s="24"/>
-      <c r="D30" s="24" t="s">
+      <c r="A30" s="18"/>
+      <c r="B30" s="18"/>
+      <c r="C30" s="18"/>
+      <c r="D30" s="18" t="s">
         <v>117</v>
       </c>
-      <c r="E30" s="24" t="s">
+      <c r="E30" s="18" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="24" t="s">
+      <c r="A31" s="18" t="s">
         <v>118</v>
       </c>
-      <c r="B31" s="24" t="s">
+      <c r="B31" s="18" t="s">
         <v>81</v>
       </c>
-      <c r="C31" s="24" t="s">
+      <c r="C31" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="D31" s="24" t="s">
+      <c r="D31" s="18" t="s">
         <v>116</v>
       </c>
-      <c r="E31" s="24" t="s">
+      <c r="E31" s="18" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="24"/>
-      <c r="B32" s="24"/>
-      <c r="C32" s="24"/>
-      <c r="D32" s="24" t="s">
+      <c r="A32" s="18"/>
+      <c r="B32" s="18"/>
+      <c r="C32" s="18"/>
+      <c r="D32" s="18" t="s">
         <v>117</v>
       </c>
-      <c r="E32" s="24" t="s">
+      <c r="E32" s="18" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="24" t="s">
+      <c r="A33" s="18" t="s">
         <v>119</v>
       </c>
-      <c r="B33" s="24" t="s">
+      <c r="B33" s="18" t="s">
         <v>72</v>
       </c>
-      <c r="C33" s="24" t="s">
+      <c r="C33" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="D33" s="24" t="s">
+      <c r="D33" s="18" t="s">
         <v>116</v>
       </c>
-      <c r="E33" s="24" t="s">
+      <c r="E33" s="18" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="24"/>
-      <c r="B34" s="24"/>
-      <c r="C34" s="24"/>
-      <c r="D34" s="24" t="s">
+      <c r="A34" s="18"/>
+      <c r="B34" s="18"/>
+      <c r="C34" s="18"/>
+      <c r="D34" s="18" t="s">
         <v>117</v>
       </c>
-      <c r="E34" s="24" t="s">
+      <c r="E34" s="18" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="24" t="s">
+      <c r="A35" s="18" t="s">
         <v>120</v>
       </c>
-      <c r="B35" s="24" t="s">
+      <c r="B35" s="18" t="s">
         <v>68</v>
       </c>
-      <c r="C35" s="24" t="s">
+      <c r="C35" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="D35" s="24" t="s">
+      <c r="D35" s="18" t="s">
         <v>121</v>
       </c>
-      <c r="E35" s="24" t="s">
+      <c r="E35" s="18" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="24"/>
-      <c r="B36" s="24"/>
-      <c r="C36" s="24"/>
-      <c r="D36" s="24" t="s">
+      <c r="A36" s="18"/>
+      <c r="B36" s="18"/>
+      <c r="C36" s="18"/>
+      <c r="D36" s="18" t="s">
         <v>117</v>
       </c>
-      <c r="E36" s="24" t="s">
+      <c r="E36" s="18" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="24" t="s">
+      <c r="A37" s="18" t="s">
         <v>122</v>
       </c>
-      <c r="B37" s="24" t="s">
+      <c r="B37" s="18" t="s">
         <v>78</v>
       </c>
-      <c r="C37" s="24" t="s">
+      <c r="C37" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="D37" s="24" t="s">
+      <c r="D37" s="18" t="s">
         <v>121</v>
       </c>
-      <c r="E37" s="24" t="s">
+      <c r="E37" s="18" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="24"/>
-      <c r="B38" s="24"/>
-      <c r="C38" s="24"/>
-      <c r="D38" s="24" t="s">
+      <c r="A38" s="18"/>
+      <c r="B38" s="18"/>
+      <c r="C38" s="18"/>
+      <c r="D38" s="18" t="s">
         <v>117</v>
       </c>
-      <c r="E38" s="24" t="s">
+      <c r="E38" s="18" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="24" t="s">
+      <c r="A39" s="18" t="s">
         <v>123</v>
       </c>
-      <c r="B39" s="24" t="s">
+      <c r="B39" s="18" t="s">
         <v>104</v>
       </c>
-      <c r="C39" s="24" t="s">
+      <c r="C39" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="D39" s="24" t="s">
+      <c r="D39" s="18" t="s">
         <v>121</v>
       </c>
-      <c r="E39" s="24" t="s">
+      <c r="E39" s="18" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="24"/>
-      <c r="B40" s="24"/>
-      <c r="C40" s="24"/>
-      <c r="D40" s="24" t="s">
+      <c r="A40" s="18"/>
+      <c r="B40" s="18"/>
+      <c r="C40" s="18"/>
+      <c r="D40" s="18" t="s">
         <v>117</v>
       </c>
-      <c r="E40" s="24" t="s">
+      <c r="E40" s="18" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="24" t="s">
+      <c r="A41" s="18" t="s">
         <v>124</v>
       </c>
-      <c r="B41" s="24" t="s">
+      <c r="B41" s="18" t="s">
         <v>125</v>
       </c>
-      <c r="C41" s="24" t="s">
+      <c r="C41" s="18" t="s">
         <v>126</v>
       </c>
-      <c r="D41" s="24" t="s">
+      <c r="D41" s="18" t="s">
         <v>117</v>
       </c>
-      <c r="E41" s="24" t="s">
+      <c r="E41" s="18" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="24" t="s">
+      <c r="A42" s="18" t="s">
         <v>127</v>
       </c>
-      <c r="B42" s="24" t="s">
+      <c r="B42" s="18" t="s">
         <v>92</v>
       </c>
-      <c r="C42" s="24" t="s">
+      <c r="C42" s="18" t="s">
         <v>84</v>
       </c>
-      <c r="D42" s="24" t="s">
+      <c r="D42" s="18" t="s">
         <v>117</v>
       </c>
-      <c r="E42" s="24" t="s">
+      <c r="E42" s="18" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="24" t="s">
+      <c r="A43" s="18" t="s">
         <v>128</v>
       </c>
-      <c r="B43" s="24" t="s">
+      <c r="B43" s="18" t="s">
         <v>129</v>
       </c>
-      <c r="C43" s="24" t="s">
+      <c r="C43" s="18" t="s">
         <v>75</v>
       </c>
-      <c r="D43" s="24" t="s">
+      <c r="D43" s="18" t="s">
         <v>117</v>
       </c>
-      <c r="E43" s="24" t="s">
+      <c r="E43" s="18" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="24" t="s">
+      <c r="A44" s="18" t="s">
         <v>116</v>
       </c>
-      <c r="B44" s="24" t="s">
+      <c r="B44" s="18" t="s">
         <v>108</v>
       </c>
-      <c r="C44" s="24" t="s">
+      <c r="C44" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="D44" s="24" t="s">
+      <c r="D44" s="18" t="s">
         <v>117</v>
       </c>
-      <c r="E44" s="24" t="s">
+      <c r="E44" s="18" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" s="24" t="s">
+      <c r="A45" s="18" t="s">
         <v>130</v>
       </c>
-      <c r="B45" s="24" t="s">
+      <c r="B45" s="18" t="s">
         <v>131</v>
       </c>
-      <c r="C45" s="24" t="s">
+      <c r="C45" s="18" t="s">
         <v>132</v>
       </c>
-      <c r="D45" s="24" t="s">
+      <c r="D45" s="18" t="s">
         <v>133</v>
       </c>
-      <c r="E45" s="24" t="s">
+      <c r="E45" s="18" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" s="24"/>
-      <c r="B46" s="24"/>
-      <c r="C46" s="24"/>
-      <c r="D46" s="24" t="s">
+      <c r="A46" s="18"/>
+      <c r="B46" s="18"/>
+      <c r="C46" s="18"/>
+      <c r="D46" s="18" t="s">
         <v>117</v>
       </c>
-      <c r="E46" s="24" t="s">
+      <c r="E46" s="18" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" s="24" t="s">
+      <c r="A47" s="18" t="s">
         <v>134</v>
       </c>
-      <c r="B47" s="24" t="s">
+      <c r="B47" s="18" t="s">
         <v>135</v>
       </c>
-      <c r="C47" s="24" t="s">
+      <c r="C47" s="18" t="s">
         <v>132</v>
       </c>
-      <c r="D47" s="24" t="s">
+      <c r="D47" s="18" t="s">
         <v>133</v>
       </c>
-      <c r="E47" s="24" t="s">
+      <c r="E47" s="18" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" s="24"/>
-      <c r="B48" s="24"/>
-      <c r="C48" s="24"/>
-      <c r="D48" s="24" t="s">
+      <c r="A48" s="18"/>
+      <c r="B48" s="18"/>
+      <c r="C48" s="18"/>
+      <c r="D48" s="18" t="s">
         <v>117</v>
       </c>
-      <c r="E48" s="24" t="s">
+      <c r="E48" s="18" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" s="24" t="s">
+      <c r="A49" s="18" t="s">
         <v>136</v>
       </c>
-      <c r="B49" s="24" t="s">
+      <c r="B49" s="18" t="s">
         <v>98</v>
       </c>
-      <c r="C49" s="24" t="s">
+      <c r="C49" s="18" t="s">
         <v>102</v>
       </c>
-      <c r="D49" s="24" t="s">
+      <c r="D49" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="E49" s="24" t="s">
+      <c r="E49" s="18" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" s="24" t="s">
+      <c r="A50" s="18" t="s">
         <v>138</v>
       </c>
-      <c r="B50" s="24" t="s">
+      <c r="B50" s="18" t="s">
         <v>98</v>
       </c>
-      <c r="C50" s="24" t="s">
+      <c r="C50" s="18" t="s">
         <v>97</v>
       </c>
-      <c r="D50" s="24" t="s">
+      <c r="D50" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="E50" s="24" t="s">
+      <c r="E50" s="18" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" s="24" t="s">
+      <c r="A51" s="18" t="s">
         <v>139</v>
       </c>
-      <c r="B51" s="24" t="s">
+      <c r="B51" s="18" t="s">
         <v>104</v>
       </c>
-      <c r="C51" s="24" t="s">
+      <c r="C51" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="D51" s="24" t="s">
+      <c r="D51" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="E51" s="24" t="s">
+      <c r="E51" s="18" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52" s="24" t="s">
+      <c r="A52" s="18" t="s">
         <v>140</v>
       </c>
-      <c r="B52" s="24" t="s">
+      <c r="B52" s="18" t="s">
         <v>89</v>
       </c>
-      <c r="C52" s="24" t="s">
+      <c r="C52" s="18" t="s">
         <v>92</v>
       </c>
-      <c r="D52" s="24" t="s">
+      <c r="D52" s="18" t="s">
         <v>141</v>
       </c>
-      <c r="E52" s="24" t="s">
+      <c r="E52" s="18" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" s="24" t="s">
+      <c r="A53" s="18" t="s">
         <v>243</v>
       </c>
-      <c r="B53" s="24" t="s">
+      <c r="B53" s="18" t="s">
         <v>95</v>
       </c>
-      <c r="C53" s="24" t="s">
+      <c r="C53" s="18" t="s">
         <v>84</v>
       </c>
-      <c r="D53" s="24" t="s">
+      <c r="D53" s="18" t="s">
         <v>141</v>
       </c>
-      <c r="E53" s="24" t="s">
+      <c r="E53" s="18" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54" s="24" t="s">
+      <c r="A54" s="18" t="s">
         <v>142</v>
       </c>
-      <c r="B54" s="24" t="s">
+      <c r="B54" s="18" t="s">
         <v>89</v>
       </c>
-      <c r="C54" s="24" t="s">
+      <c r="C54" s="18" t="s">
         <v>81</v>
       </c>
-      <c r="D54" s="24" t="s">
+      <c r="D54" s="18" t="s">
         <v>143</v>
       </c>
-      <c r="E54" s="24" t="s">
+      <c r="E54" s="18" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55" s="24" t="s">
+      <c r="A55" s="18" t="s">
         <v>144</v>
       </c>
-      <c r="B55" s="24" t="s">
+      <c r="B55" s="18" t="s">
         <v>81</v>
       </c>
-      <c r="C55" s="24" t="s">
+      <c r="C55" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="D55" s="24" t="s">
+      <c r="D55" s="18" t="s">
         <v>145</v>
       </c>
-      <c r="E55" s="24" t="s">
+      <c r="E55" s="18" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A56" s="24" t="s">
+      <c r="A56" s="18" t="s">
         <v>146</v>
       </c>
-      <c r="B56" s="24" t="s">
+      <c r="B56" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="C56" s="24" t="s">
+      <c r="C56" s="18" t="s">
         <v>84</v>
       </c>
-      <c r="D56" s="24" t="s">
+      <c r="D56" s="18" t="s">
         <v>147</v>
       </c>
-      <c r="E56" s="24"/>
+      <c r="E56" s="18"/>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A57" s="24" t="s">
+      <c r="A57" s="18" t="s">
         <v>148</v>
       </c>
-      <c r="B57" s="24" t="s">
+      <c r="B57" s="18" t="s">
         <v>81</v>
       </c>
-      <c r="C57" s="24" t="s">
+      <c r="C57" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="D57" s="24" t="s">
+      <c r="D57" s="18" t="s">
         <v>149</v>
       </c>
-      <c r="E57" s="24"/>
+      <c r="E57" s="18"/>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A58" s="24" t="s">
+      <c r="A58" s="18" t="s">
         <v>150</v>
       </c>
-      <c r="B58" s="24" t="s">
+      <c r="B58" s="18" t="s">
         <v>78</v>
       </c>
-      <c r="C58" s="24" t="s">
+      <c r="C58" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="D58" s="24" t="s">
+      <c r="D58" s="18" t="s">
         <v>151</v>
       </c>
-      <c r="E58" s="24"/>
+      <c r="E58" s="18"/>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A59" s="24" t="s">
+      <c r="A59" s="18" t="s">
         <v>152</v>
       </c>
-      <c r="B59" s="24" t="s">
+      <c r="B59" s="18" t="s">
         <v>75</v>
       </c>
-      <c r="C59" s="24" t="s">
+      <c r="C59" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="D59" s="24" t="s">
+      <c r="D59" s="18" t="s">
         <v>153</v>
       </c>
-      <c r="E59" s="24"/>
+      <c r="E59" s="18"/>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A60" s="24" t="s">
+      <c r="A60" s="18" t="s">
         <v>154</v>
       </c>
-      <c r="B60" s="24" t="s">
+      <c r="B60" s="18" t="s">
         <v>72</v>
       </c>
-      <c r="C60" s="24" t="s">
+      <c r="C60" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="D60" s="24" t="s">
+      <c r="D60" s="18" t="s">
         <v>155</v>
       </c>
-      <c r="E60" s="24"/>
+      <c r="E60" s="18"/>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A61" s="24" t="s">
+      <c r="A61" s="18" t="s">
         <v>156</v>
       </c>
-      <c r="B61" s="24" t="s">
+      <c r="B61" s="18" t="s">
         <v>68</v>
       </c>
-      <c r="C61" s="24" t="s">
+      <c r="C61" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="D61" s="24" t="s">
+      <c r="D61" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="E61" s="24"/>
+      <c r="E61" s="18"/>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A62" s="16"/>
-      <c r="B62" s="16"/>
-      <c r="C62" s="16"/>
-      <c r="D62" s="16"/>
-      <c r="E62" s="16"/>
+      <c r="A62" s="1"/>
+      <c r="B62" s="1"/>
+      <c r="C62" s="1"/>
+      <c r="D62" s="1"/>
+      <c r="E62" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -2980,10 +2991,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8890B3F8-F83B-4EBC-AA4A-7C0E8C96EFBF}">
-  <dimension ref="A1:E80"/>
+  <dimension ref="A1:E82"/>
   <sheetViews>
-    <sheetView topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="D96" sqref="D96"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="D55" activeCellId="3" sqref="D68 D63 D60 D55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2995,1272 +3006,1306 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="C1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="D1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="17" t="s">
+      <c r="E1" s="5" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="13" t="s">
         <v>157</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="13" t="s">
         <v>158</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="C2" s="13" t="s">
         <v>159</v>
       </c>
-      <c r="D2" s="25" t="s">
+      <c r="D2" s="19" t="s">
         <v>143</v>
       </c>
-      <c r="E2" s="15" t="s">
+      <c r="E2" s="13" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="8" t="s">
         <v>161</v>
       </c>
-      <c r="B3" s="19" t="s">
+      <c r="B3" s="8" t="s">
         <v>108</v>
       </c>
-      <c r="C3" s="19" t="s">
+      <c r="C3" s="8" t="s">
         <v>158</v>
       </c>
-      <c r="D3" s="19" t="s">
+      <c r="D3" s="8" t="s">
         <v>162</v>
       </c>
-      <c r="E3" s="19" t="s">
+      <c r="E3" s="8" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="19"/>
-      <c r="B4" s="19"/>
-      <c r="C4" s="19"/>
-      <c r="D4" s="19" t="s">
+      <c r="A4" s="8"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8" t="s">
         <v>143</v>
       </c>
-      <c r="E4" s="19" t="s">
+      <c r="E4" s="8" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="19" t="s">
+      <c r="A5" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="B5" s="19" t="s">
+      <c r="B5" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="C5" s="19" t="s">
+      <c r="C5" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="D5" s="19" t="s">
+      <c r="D5" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="E5" s="19" t="s">
+      <c r="E5" s="8" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="19" t="s">
+      <c r="A6" s="8" t="s">
         <v>163</v>
       </c>
-      <c r="B6" s="19" t="s">
+      <c r="B6" s="8" t="s">
         <v>164</v>
       </c>
-      <c r="C6" s="19" t="s">
+      <c r="C6" s="8" t="s">
         <v>158</v>
       </c>
-      <c r="D6" s="19" t="s">
+      <c r="D6" s="8" t="s">
         <v>162</v>
       </c>
-      <c r="E6" s="19" t="s">
+      <c r="E6" s="8" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="19" t="s">
+      <c r="A7" s="8" t="s">
         <v>165</v>
       </c>
-      <c r="B7" s="19" t="s">
+      <c r="B7" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="C7" s="19" t="s">
+      <c r="C7" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="19" t="s">
+      <c r="D7" s="8" t="s">
         <v>143</v>
       </c>
-      <c r="E7" s="19" t="s">
+      <c r="E7" s="8" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="19" t="s">
+      <c r="A8" s="8" t="s">
         <v>166</v>
       </c>
-      <c r="B8" s="19" t="s">
+      <c r="B8" s="8" t="s">
         <v>167</v>
       </c>
-      <c r="C8" s="19" t="s">
+      <c r="C8" s="8" t="s">
         <v>168</v>
       </c>
-      <c r="D8" s="19" t="s">
+      <c r="D8" s="8" t="s">
         <v>169</v>
       </c>
-      <c r="E8" s="19" t="s">
+      <c r="E8" s="8" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="19"/>
-      <c r="B9" s="19"/>
-      <c r="C9" s="19"/>
-      <c r="D9" s="19" t="s">
+      <c r="A9" s="8"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8" t="s">
         <v>143</v>
       </c>
-      <c r="E9" s="19" t="s">
+      <c r="E9" s="8" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="19" t="s">
+      <c r="A10" s="8" t="s">
         <v>170</v>
       </c>
-      <c r="B10" s="19" t="s">
+      <c r="B10" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="C10" s="19" t="s">
+      <c r="C10" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="D10" s="19" t="s">
+      <c r="D10" s="8" t="s">
         <v>143</v>
       </c>
-      <c r="E10" s="19" t="s">
+      <c r="E10" s="8" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="19" t="s">
+      <c r="A11" s="8" t="s">
         <v>171</v>
       </c>
-      <c r="B11" s="19" t="s">
+      <c r="B11" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="C11" s="19" t="s">
+      <c r="C11" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="D11" s="19" t="s">
+      <c r="D11" s="8" t="s">
         <v>143</v>
       </c>
-      <c r="E11" s="19" t="s">
+      <c r="E11" s="8" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="19" t="s">
+      <c r="A12" s="8" t="s">
         <v>172</v>
       </c>
-      <c r="B12" s="19" t="s">
+      <c r="B12" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C12" s="19" t="s">
+      <c r="C12" s="8" t="s">
         <v>168</v>
       </c>
-      <c r="D12" s="19" t="s">
+      <c r="D12" s="8" t="s">
         <v>169</v>
       </c>
-      <c r="E12" s="19" t="s">
+      <c r="E12" s="8" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="19"/>
-      <c r="B13" s="19"/>
-      <c r="C13" s="19"/>
-      <c r="D13" s="19" t="s">
+      <c r="A13" s="8"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8" t="s">
         <v>143</v>
       </c>
-      <c r="E13" s="19" t="s">
+      <c r="E13" s="8" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="19" t="s">
+      <c r="A14" s="8" t="s">
         <v>173</v>
       </c>
-      <c r="B14" s="19" t="s">
+      <c r="B14" s="8" t="s">
         <v>174</v>
       </c>
-      <c r="C14" s="19" t="s">
+      <c r="C14" s="8" t="s">
         <v>164</v>
       </c>
-      <c r="D14" s="19" t="s">
+      <c r="D14" s="8" t="s">
         <v>175</v>
       </c>
-      <c r="E14" s="19" t="s">
+      <c r="E14" s="8" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="19"/>
-      <c r="B15" s="19"/>
-      <c r="C15" s="19"/>
-      <c r="D15" s="19" t="s">
+      <c r="A15" s="8"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8" t="s">
         <v>176</v>
       </c>
-      <c r="E15" s="19" t="s">
+      <c r="E15" s="8" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="19" t="s">
+      <c r="A16" s="8" t="s">
         <v>177</v>
       </c>
-      <c r="B16" s="19" t="s">
+      <c r="B16" s="8" t="s">
         <v>178</v>
       </c>
-      <c r="C16" s="19" t="s">
+      <c r="C16" s="8" t="s">
         <v>164</v>
       </c>
-      <c r="D16" s="19" t="s">
+      <c r="D16" s="8" t="s">
         <v>175</v>
       </c>
-      <c r="E16" s="19" t="s">
+      <c r="E16" s="8" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="19"/>
-      <c r="B17" s="19"/>
-      <c r="C17" s="19"/>
-      <c r="D17" s="19" t="s">
+      <c r="A17" s="8"/>
+      <c r="B17" s="8"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8" t="s">
         <v>176</v>
       </c>
-      <c r="E17" s="19" t="s">
+      <c r="E17" s="8" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="19" t="s">
+      <c r="A18" s="8" t="s">
         <v>179</v>
       </c>
-      <c r="B18" s="19" t="s">
+      <c r="B18" s="8" t="s">
         <v>180</v>
       </c>
-      <c r="C18" s="19" t="s">
+      <c r="C18" s="8" t="s">
         <v>164</v>
       </c>
-      <c r="D18" s="19" t="s">
+      <c r="D18" s="8" t="s">
         <v>175</v>
       </c>
-      <c r="E18" s="19" t="s">
+      <c r="E18" s="8" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="19"/>
-      <c r="B19" s="19"/>
-      <c r="C19" s="19"/>
-      <c r="D19" s="19" t="s">
+      <c r="A19" s="8"/>
+      <c r="B19" s="8"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="8" t="s">
         <v>176</v>
       </c>
-      <c r="E19" s="19" t="s">
+      <c r="E19" s="8" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="19" t="s">
+      <c r="A20" s="8" t="s">
         <v>181</v>
       </c>
-      <c r="B20" s="19" t="s">
+      <c r="B20" s="8" t="s">
         <v>182</v>
       </c>
-      <c r="C20" s="19" t="s">
+      <c r="C20" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="D20" s="19" t="s">
+      <c r="D20" s="8" t="s">
         <v>117</v>
       </c>
-      <c r="E20" s="19" t="s">
+      <c r="E20" s="8" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="19" t="s">
+      <c r="A21" s="8" t="s">
         <v>183</v>
       </c>
-      <c r="B21" s="19" t="s">
+      <c r="B21" s="8" t="s">
         <v>184</v>
       </c>
-      <c r="C21" s="19" t="s">
+      <c r="C21" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="D21" s="19" t="s">
+      <c r="D21" s="8" t="s">
         <v>117</v>
       </c>
-      <c r="E21" s="19" t="s">
+      <c r="E21" s="8" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="19" t="s">
+      <c r="A22" s="8" t="s">
         <v>185</v>
       </c>
-      <c r="B22" s="19" t="s">
+      <c r="B22" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="C22" s="19" t="s">
+      <c r="C22" s="8" t="s">
         <v>186</v>
       </c>
-      <c r="D22" s="19" t="s">
+      <c r="D22" s="8" t="s">
         <v>117</v>
       </c>
-      <c r="E22" s="19" t="s">
+      <c r="E22" s="8" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="19" t="s">
+      <c r="A23" s="8" t="s">
         <v>187</v>
       </c>
-      <c r="B23" s="19" t="s">
+      <c r="B23" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="C23" s="19" t="s">
+      <c r="C23" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="D23" s="19" t="s">
+      <c r="D23" s="8" t="s">
         <v>188</v>
       </c>
-      <c r="E23" s="19" t="s">
+      <c r="E23" s="8" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="19"/>
-      <c r="B24" s="19"/>
-      <c r="C24" s="19"/>
-      <c r="D24" s="19" t="s">
+      <c r="A24" s="8"/>
+      <c r="B24" s="8"/>
+      <c r="C24" s="8"/>
+      <c r="D24" s="8" t="s">
         <v>189</v>
       </c>
-      <c r="E24" s="19" t="s">
+      <c r="E24" s="8" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="19" t="s">
+      <c r="A25" s="8" t="s">
         <v>190</v>
       </c>
-      <c r="B25" s="19" t="s">
+      <c r="B25" s="8" t="s">
         <v>191</v>
       </c>
-      <c r="C25" s="19" t="s">
+      <c r="C25" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="D25" s="19" t="s">
+      <c r="D25" s="8" t="s">
         <v>188</v>
       </c>
-      <c r="E25" s="19" t="s">
+      <c r="E25" s="8" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="19"/>
-      <c r="B26" s="19"/>
-      <c r="C26" s="19"/>
-      <c r="D26" s="19" t="s">
+      <c r="A26" s="8"/>
+      <c r="B26" s="8"/>
+      <c r="C26" s="8"/>
+      <c r="D26" s="8" t="s">
         <v>189</v>
       </c>
-      <c r="E26" s="19" t="s">
+      <c r="E26" s="8" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="19" t="s">
+      <c r="A27" s="8" t="s">
         <v>192</v>
       </c>
-      <c r="B27" s="19" t="s">
+      <c r="B27" s="8" t="s">
         <v>184</v>
       </c>
-      <c r="C27" s="19" t="s">
+      <c r="C27" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="D27" s="19" t="s">
+      <c r="D27" s="8" t="s">
         <v>188</v>
       </c>
-      <c r="E27" s="19" t="s">
+      <c r="E27" s="8" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="19"/>
-      <c r="B28" s="19"/>
-      <c r="C28" s="19"/>
-      <c r="D28" s="19" t="s">
+      <c r="A28" s="8"/>
+      <c r="B28" s="8"/>
+      <c r="C28" s="8"/>
+      <c r="D28" s="8" t="s">
         <v>193</v>
       </c>
-      <c r="E28" s="19" t="s">
+      <c r="E28" s="8" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="19" t="s">
+      <c r="A29" s="8" t="s">
         <v>194</v>
       </c>
-      <c r="B29" s="19" t="s">
+      <c r="B29" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="C29" s="19" t="s">
+      <c r="C29" s="8" t="s">
         <v>184</v>
       </c>
-      <c r="D29" s="19" t="s">
+      <c r="D29" s="8" t="s">
         <v>195</v>
       </c>
-      <c r="E29" s="19" t="s">
+      <c r="E29" s="8" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="19" t="s">
+      <c r="A30" s="8" t="s">
         <v>196</v>
       </c>
-      <c r="B30" s="19" t="s">
+      <c r="B30" s="8" t="s">
         <v>197</v>
       </c>
-      <c r="C30" s="19" t="s">
+      <c r="C30" s="8" t="s">
         <v>198</v>
       </c>
-      <c r="D30" s="19" t="s">
+      <c r="D30" s="8" t="s">
         <v>195</v>
       </c>
-      <c r="E30" s="19" t="s">
+      <c r="E30" s="8" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="19" t="s">
+      <c r="A31" s="8" t="s">
         <v>199</v>
       </c>
-      <c r="B31" s="19" t="s">
+      <c r="B31" s="8" t="s">
         <v>168</v>
       </c>
-      <c r="C31" s="19" t="s">
+      <c r="C31" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="D31" s="19" t="s">
+      <c r="D31" s="8" t="s">
         <v>200</v>
       </c>
-      <c r="E31" s="19" t="s">
+      <c r="E31" s="8" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="19"/>
-      <c r="B32" s="19"/>
-      <c r="C32" s="19"/>
-      <c r="D32" s="19" t="s">
+      <c r="A32" s="8"/>
+      <c r="B32" s="8"/>
+      <c r="C32" s="8"/>
+      <c r="D32" s="8" t="s">
         <v>201</v>
       </c>
-      <c r="E32" s="19" t="s">
+      <c r="E32" s="8" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="19" t="s">
+      <c r="A33" s="8" t="s">
         <v>202</v>
       </c>
-      <c r="B33" s="19" t="s">
+      <c r="B33" s="8" t="s">
         <v>158</v>
       </c>
-      <c r="C33" s="19" t="s">
+      <c r="C33" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="D33" s="19" t="s">
+      <c r="D33" s="8" t="s">
         <v>200</v>
       </c>
-      <c r="E33" s="19" t="s">
+      <c r="E33" s="8" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="19"/>
-      <c r="B34" s="19"/>
-      <c r="C34" s="19"/>
-      <c r="D34" s="19" t="s">
+      <c r="A34" s="8"/>
+      <c r="B34" s="8"/>
+      <c r="C34" s="8"/>
+      <c r="D34" s="8" t="s">
         <v>201</v>
       </c>
-      <c r="E34" s="19" t="s">
+      <c r="E34" s="8" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="19" t="s">
+      <c r="A35" s="8" t="s">
         <v>203</v>
       </c>
-      <c r="B35" s="19" t="s">
+      <c r="B35" s="8" t="s">
         <v>204</v>
       </c>
-      <c r="C35" s="19" t="s">
+      <c r="C35" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="D35" s="19" t="s">
+      <c r="D35" s="8" t="s">
         <v>201</v>
       </c>
-      <c r="E35" s="19" t="s">
+      <c r="E35" s="8" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="19" t="s">
+      <c r="A36" s="8" t="s">
         <v>205</v>
       </c>
-      <c r="B36" s="19" t="s">
+      <c r="B36" s="8" t="s">
         <v>206</v>
       </c>
-      <c r="C36" s="19" t="s">
+      <c r="C36" s="8" t="s">
         <v>204</v>
       </c>
-      <c r="D36" s="19" t="s">
+      <c r="D36" s="8" t="s">
         <v>207</v>
       </c>
-      <c r="E36" s="19" t="s">
+      <c r="E36" s="8" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="19" t="s">
+      <c r="A37" s="8" t="s">
         <v>208</v>
       </c>
-      <c r="B37" s="19" t="s">
+      <c r="B37" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="C37" s="19" t="s">
+      <c r="C37" s="8" t="s">
         <v>204</v>
       </c>
-      <c r="D37" s="19" t="s">
+      <c r="D37" s="8" t="s">
         <v>207</v>
       </c>
-      <c r="E37" s="19" t="s">
+      <c r="E37" s="8" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="19" t="s">
+      <c r="A38" s="8" t="s">
         <v>209</v>
       </c>
-      <c r="B38" s="19" t="s">
+      <c r="B38" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="C38" s="19" t="s">
+      <c r="C38" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="D38" s="19" t="s">
+      <c r="D38" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="E38" s="19" t="s">
+      <c r="E38" s="8" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="19" t="s">
+      <c r="A39" s="8" t="s">
         <v>210</v>
       </c>
-      <c r="B39" s="19" t="s">
+      <c r="B39" s="8" t="s">
         <v>182</v>
       </c>
-      <c r="C39" s="19" t="s">
+      <c r="C39" s="8" t="s">
         <v>167</v>
       </c>
-      <c r="D39" s="19" t="s">
+      <c r="D39" s="8" t="s">
         <v>211</v>
       </c>
-      <c r="E39" s="19" t="s">
+      <c r="E39" s="8" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="19" t="s">
+      <c r="A40" s="8" t="s">
         <v>157</v>
       </c>
-      <c r="B40" s="19" t="s">
+      <c r="B40" s="8" t="s">
         <v>158</v>
       </c>
-      <c r="C40" s="19" t="s">
+      <c r="C40" s="8" t="s">
         <v>159</v>
       </c>
-      <c r="D40" s="19" t="s">
+      <c r="D40" s="8" t="s">
         <v>143</v>
       </c>
-      <c r="E40" s="19" t="s">
+      <c r="E40" s="8" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="19" t="s">
+      <c r="A41" s="8" t="s">
         <v>212</v>
       </c>
-      <c r="B41" s="19" t="s">
+      <c r="B41" s="8" t="s">
         <v>164</v>
       </c>
-      <c r="C41" s="19" t="s">
+      <c r="C41" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="D41" s="19" t="s">
+      <c r="D41" s="8" t="s">
         <v>213</v>
       </c>
-      <c r="E41" s="19" t="s">
+      <c r="E41" s="8" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="19" t="s">
+      <c r="A42" s="8" t="s">
         <v>214</v>
       </c>
-      <c r="B42" s="19" t="s">
+      <c r="B42" s="8" t="s">
         <v>215</v>
       </c>
-      <c r="C42" s="19" t="s">
+      <c r="C42" s="8" t="s">
         <v>204</v>
       </c>
-      <c r="D42" s="19" t="s">
+      <c r="D42" s="8" t="s">
         <v>143</v>
       </c>
-      <c r="E42" s="19" t="s">
+      <c r="E42" s="8" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="19" t="s">
+      <c r="A43" s="8" t="s">
         <v>216</v>
       </c>
-      <c r="B43" s="19" t="s">
+      <c r="B43" s="8" t="s">
         <v>217</v>
       </c>
-      <c r="C43" s="19" t="s">
+      <c r="C43" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="D43" s="19" t="s">
+      <c r="D43" s="8" t="s">
         <v>200</v>
       </c>
-      <c r="E43" s="19" t="s">
+      <c r="E43" s="8" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="19"/>
-      <c r="B44" s="19"/>
-      <c r="C44" s="19"/>
-      <c r="D44" s="19" t="s">
+      <c r="A44" s="8"/>
+      <c r="B44" s="8"/>
+      <c r="C44" s="8"/>
+      <c r="D44" s="8" t="s">
         <v>201</v>
       </c>
-      <c r="E44" s="19" t="s">
+      <c r="E44" s="8" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" s="19" t="s">
+      <c r="A45" s="8" t="s">
         <v>218</v>
       </c>
-      <c r="B45" s="19" t="s">
+      <c r="B45" s="8" t="s">
         <v>219</v>
       </c>
-      <c r="C45" s="19" t="s">
+      <c r="C45" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="D45" s="19" t="s">
+      <c r="D45" s="8" t="s">
         <v>200</v>
       </c>
-      <c r="E45" s="19" t="s">
+      <c r="E45" s="8" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" s="19"/>
-      <c r="B46" s="19"/>
-      <c r="C46" s="19"/>
-      <c r="D46" s="19" t="s">
+      <c r="A46" s="8"/>
+      <c r="B46" s="8"/>
+      <c r="C46" s="8"/>
+      <c r="D46" s="8" t="s">
         <v>201</v>
       </c>
-      <c r="E46" s="19" t="s">
+      <c r="E46" s="8" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" s="19" t="s">
+      <c r="A47" s="8" t="s">
         <v>220</v>
       </c>
-      <c r="B47" s="19" t="s">
+      <c r="B47" s="8" t="s">
         <v>221</v>
       </c>
-      <c r="C47" s="19" t="s">
+      <c r="C47" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="D47" s="19" t="s">
+      <c r="D47" s="8" t="s">
         <v>200</v>
       </c>
-      <c r="E47" s="19" t="s">
+      <c r="E47" s="8" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" s="19"/>
-      <c r="B48" s="19"/>
-      <c r="C48" s="19"/>
-      <c r="D48" s="19" t="s">
+      <c r="A48" s="8"/>
+      <c r="B48" s="8"/>
+      <c r="C48" s="8"/>
+      <c r="D48" s="8" t="s">
         <v>201</v>
       </c>
-      <c r="E48" s="19" t="s">
+      <c r="E48" s="8" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" s="16" t="s">
+      <c r="A49" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="B49" s="16" t="s">
+      <c r="B49" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C49" s="16" t="s">
+      <c r="C49" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="D49" s="16" t="s">
+      <c r="D49" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="E49" s="16" t="s">
+      <c r="E49" s="1" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" s="16" t="s">
+      <c r="A50" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="B50" s="16" t="s">
+      <c r="B50" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="C50" s="16" t="s">
+      <c r="C50" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="D50" s="16" t="s">
+      <c r="D50" s="21" t="s">
         <v>90</v>
       </c>
-      <c r="E50" s="16" t="s">
+      <c r="E50" s="1" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" s="16" t="s">
+      <c r="A51" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="B51" s="16" t="s">
+      <c r="B51" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="C51" s="16" t="s">
+      <c r="C51" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="D51" s="16" t="s">
+      <c r="D51" s="21" t="s">
         <v>90</v>
       </c>
-      <c r="E51" s="16" t="s">
+      <c r="E51" s="1" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52" s="16" t="s">
+      <c r="A52" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="B52" s="16" t="s">
+      <c r="B52" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="C52" s="16" t="s">
+      <c r="C52" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="D52" s="16" t="s">
+      <c r="D52" s="21" t="s">
         <v>90</v>
       </c>
-      <c r="E52" s="16" t="s">
+      <c r="E52" s="1" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" s="16" t="s">
+      <c r="A53" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="B53" s="16" t="s">
+      <c r="B53" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C53" s="16" t="s">
+      <c r="C53" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="D53" s="16" t="s">
+      <c r="D53" s="21" t="s">
         <v>90</v>
       </c>
-      <c r="E53" s="16" t="s">
+      <c r="E53" s="1" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54" s="16" t="s">
+      <c r="A54" s="1" t="s">
         <v>227</v>
       </c>
-      <c r="B54" s="16" t="s">
+      <c r="B54" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="C54" s="16" t="s">
+      <c r="C54" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="D54" s="16" t="s">
+      <c r="D54" s="21" t="s">
         <v>90</v>
       </c>
-      <c r="E54" s="16" t="s">
+      <c r="E54" s="1" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55" s="16" t="s">
+      <c r="A55" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="B55" s="16" t="s">
+      <c r="B55" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="C55" s="16" t="s">
+      <c r="C55" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="D55" s="16" t="s">
+      <c r="D55" s="21" t="s">
         <v>90</v>
       </c>
-      <c r="E55" s="16" t="s">
+      <c r="E55" s="1" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A56" s="16" t="s">
+      <c r="A56" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="B56" s="16" t="s">
+      <c r="B56" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="C56" s="16" t="s">
+      <c r="C56" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="D56" s="16" t="s">
+      <c r="D56" s="21" t="s">
         <v>90</v>
       </c>
-      <c r="E56" s="16" t="s">
+      <c r="E56" s="1" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A57" s="16" t="s">
+      <c r="A57" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="B57" s="16" t="s">
+      <c r="B57" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="C57" s="16" t="s">
+      <c r="C57" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D57" s="16" t="s">
+      <c r="D57" s="21" t="s">
         <v>90</v>
       </c>
-      <c r="E57" s="16" t="s">
+      <c r="E57" s="1" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A58" s="16" t="s">
+      <c r="A58" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="B58" s="16" t="s">
+      <c r="B58" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="C58" s="16" t="s">
+      <c r="C58" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="D58" s="16" t="s">
+      <c r="D58" s="21" t="s">
         <v>90</v>
       </c>
-      <c r="E58" s="16" t="s">
+      <c r="E58" s="1" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A59" s="16" t="s">
+      <c r="A59" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="B59" s="16" t="s">
+      <c r="B59" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C59" s="16" t="s">
+      <c r="C59" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="D59" s="16" t="s">
+      <c r="D59" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="E59" s="16" t="s">
+      <c r="E59" s="1" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A60" s="16" t="s">
+      <c r="A60" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="B60" s="16" t="s">
+      <c r="B60" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="C60" s="16" t="s">
+      <c r="C60" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D60" s="16" t="s">
+      <c r="D60" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="E60" s="16" t="s">
+      <c r="E60" s="1" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A61" s="16" t="s">
+      <c r="A61" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="B61" s="16" t="s">
+      <c r="B61" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C61" s="16" t="s">
+      <c r="C61" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="D61" s="16" t="s">
+      <c r="D61" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="E61" s="16" t="s">
+      <c r="E61" s="1" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A62" s="16" t="s">
+      <c r="A62" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="B62" s="16" t="s">
+      <c r="B62" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="C62" s="16" t="s">
+      <c r="C62" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="D62" s="16" t="s">
+      <c r="D62" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="E62" s="16" t="s">
+      <c r="E62" s="1" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A63" s="16" t="s">
+      <c r="A63" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="B63" s="16" t="s">
+      <c r="B63" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="C63" s="16" t="s">
+      <c r="C63" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="D63" s="16" t="s">
+      <c r="D63" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="E63" s="16" t="s">
+      <c r="E63" s="1" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A64" s="16" t="s">
+      <c r="A64" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="B64" s="16" t="s">
+      <c r="B64" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C64" s="16" t="s">
+      <c r="C64" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="D64" s="16" t="s">
+      <c r="D64" s="21" t="s">
         <v>238</v>
       </c>
-      <c r="E64" s="16" t="s">
+      <c r="E64" s="1" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A65" s="16" t="s">
+      <c r="A65" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="B65" s="16" t="s">
+      <c r="B65" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="C65" s="16" t="s">
+      <c r="C65" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="D65" s="16" t="s">
+      <c r="D65" s="21" t="s">
         <v>240</v>
       </c>
-      <c r="E65" s="16" t="s">
+      <c r="E65" s="1" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A66" s="16" t="s">
+      <c r="A66" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="B66" s="16" t="s">
+      <c r="B66" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="C66" s="16" t="s">
+      <c r="C66" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="D66" s="16" t="s">
+      <c r="D66" s="21" t="s">
         <v>240</v>
       </c>
-      <c r="E66" s="16" t="s">
+      <c r="E66" s="1" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A67" s="16" t="s">
+      <c r="A67" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="B67" s="16" t="s">
+      <c r="B67" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="C67" s="16" t="s">
+      <c r="C67" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="D67" s="16" t="s">
+      <c r="D67" s="21" t="s">
         <v>240</v>
       </c>
-      <c r="E67" s="16" t="s">
+      <c r="E67" s="1" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A68" s="16" t="s">
+      <c r="A68" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="B68" s="16" t="s">
+      <c r="B68" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C68" s="16" t="s">
+      <c r="C68" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="D68" s="16" t="s">
+      <c r="D68" s="21" t="s">
         <v>141</v>
       </c>
-      <c r="E68" s="16" t="s">
+      <c r="E68" s="1" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A69" s="16" t="s">
+      <c r="A69" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="B69" s="16" t="s">
+      <c r="B69" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="C69" s="16" t="s">
+      <c r="C69" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="D69" s="16" t="s">
+      <c r="D69" s="21" t="s">
         <v>245</v>
       </c>
-      <c r="E69" s="16" t="s">
+      <c r="E69" s="1" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A70" s="16" t="s">
+      <c r="A70" s="1" t="s">
         <v>246</v>
       </c>
-      <c r="B70" s="16" t="s">
+      <c r="B70" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C70" s="16" t="s">
+      <c r="C70" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="D70" s="16" t="s">
+      <c r="D70" s="21" t="s">
         <v>247</v>
       </c>
-      <c r="E70" s="16" t="s">
+      <c r="E70" s="1" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A71" s="16" t="s">
+      <c r="A71" s="1" t="s">
         <v>248</v>
       </c>
-      <c r="B71" s="16" t="s">
+      <c r="B71" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C71" s="16" t="s">
+      <c r="C71" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="D71" s="16" t="s">
+      <c r="D71" s="21" t="s">
         <v>247</v>
       </c>
-      <c r="E71" s="16" t="s">
+      <c r="E71" s="1" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A72" s="16" t="s">
+      <c r="A72" s="1" t="s">
         <v>249</v>
       </c>
-      <c r="B72" s="16" t="s">
+      <c r="B72" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C72" s="16" t="s">
+      <c r="C72" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="D72" s="16" t="s">
+      <c r="D72" s="21" t="s">
         <v>247</v>
       </c>
-      <c r="E72" s="16" t="s">
+      <c r="E72" s="1" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A73" s="16" t="s">
+      <c r="A73" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="B73" s="16" t="s">
+      <c r="B73" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C73" s="16" t="s">
+      <c r="C73" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="D73" s="16" t="s">
+      <c r="D73" s="21" t="s">
         <v>247</v>
       </c>
-      <c r="E73" s="16" t="s">
+      <c r="E73" s="1" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A74" s="16" t="s">
+      <c r="A74" s="1" t="s">
         <v>251</v>
       </c>
-      <c r="B74" s="16" t="s">
+      <c r="B74" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C74" s="16" t="s">
+      <c r="C74" s="1" t="s">
         <v>252</v>
       </c>
-      <c r="D74" s="16" t="s">
+      <c r="D74" s="21" t="s">
         <v>247</v>
       </c>
-      <c r="E74" s="16" t="s">
+      <c r="E74" s="1" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A75" s="16" t="s">
+      <c r="A75" s="1" t="s">
         <v>253</v>
       </c>
-      <c r="B75" s="16" t="s">
+      <c r="B75" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C75" s="16" t="s">
+      <c r="C75" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="D75" s="16" t="s">
+      <c r="D75" s="21" t="s">
         <v>247</v>
       </c>
-      <c r="E75" s="16" t="s">
+      <c r="E75" s="1" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A76" s="16" t="s">
+      <c r="A76" s="1" t="s">
         <v>254</v>
       </c>
-      <c r="B76" s="16" t="s">
+      <c r="B76" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="C76" s="16" t="s">
+      <c r="C76" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="D76" s="16" t="s">
+      <c r="D76" s="21" t="s">
         <v>255</v>
       </c>
-      <c r="E76" s="16" t="s">
+      <c r="E76" s="1" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A77" s="16" t="s">
+      <c r="A77" s="1" t="s">
         <v>256</v>
       </c>
-      <c r="B77" s="16" t="s">
+      <c r="B77" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C77" s="16" t="s">
+      <c r="C77" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="D77" s="16" t="s">
+      <c r="D77" s="21" t="s">
         <v>188</v>
       </c>
-      <c r="E77" s="16" t="s">
+      <c r="E77" s="1" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A78" s="16" t="s">
+      <c r="A78" s="1" t="s">
         <v>257</v>
       </c>
-      <c r="B78" s="16" t="s">
+      <c r="B78" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C78" s="26" t="s">
+      <c r="C78" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="D78" s="16" t="s">
+      <c r="D78" s="21" t="s">
         <v>193</v>
       </c>
-      <c r="E78" s="16" t="s">
+      <c r="E78" s="1" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A79" s="16"/>
-      <c r="B79" s="16"/>
-      <c r="C79" s="16"/>
-      <c r="D79" s="16" t="s">
+      <c r="A79" s="1"/>
+      <c r="B79" s="1"/>
+      <c r="C79" s="1"/>
+      <c r="D79" s="21" t="s">
         <v>188</v>
       </c>
-      <c r="E79" s="16" t="s">
+      <c r="E79" s="1" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A80" s="16" t="s">
+      <c r="A80" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="B80" s="16" t="s">
+      <c r="B80" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C80" s="16" t="s">
+      <c r="C80" s="1" t="s">
         <v>259</v>
       </c>
-      <c r="D80" s="16" t="s">
+      <c r="D80" s="21" t="s">
         <v>188</v>
       </c>
-      <c r="E80" s="16" t="s">
+      <c r="E80" s="1" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A81" s="22" t="s">
+        <v>260</v>
+      </c>
+      <c r="B81" s="22" t="s">
+        <v>204</v>
+      </c>
+      <c r="C81" s="22" t="s">
+        <v>206</v>
+      </c>
+      <c r="D81" s="21" t="s">
+        <v>261</v>
+      </c>
+      <c r="E81" s="22" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A82" s="22" t="s">
+        <v>262</v>
+      </c>
+      <c r="B82" s="22" t="s">
+        <v>198</v>
+      </c>
+      <c r="C82" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="D82" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="E82" s="22" t="s">
         <v>160</v>
       </c>
     </row>

</xml_diff>